<commit_message>
updated 5_1 - 5_5 - 7_3 excelexc_solved
</commit_message>
<xml_diff>
--- a/ZZ_Other/Exp_Smoothing_Trended_exercise.xlsx
+++ b/ZZ_Other/Exp_Smoothing_Trended_exercise.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/197ab797fdac369a/IE/2022_Fall/ZZ_Notebooks/NB_PPLE_Fall2022/Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/197ab797fdac369a/IE_Classes/2022_Fall/ZZ_Notebooks/NB_BDBA_Fall2022_Students/ZZ_Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{C707783C-04DC-41F6-A200-D4A40F1D4148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52F8B7C4-828B-4BC8-9205-C1961BE83AA9}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{C707783C-04DC-41F6-A200-D4A40F1D4148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9BC83E3-6D71-44F9-B33C-6DEF5B593A6C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E8F85D3-1CA2-4F29-ACB1-42411CDB7F52}"/>
   </bookViews>
@@ -223,6 +223,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>259616</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114409</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23C3183B-0836-16F2-2C31-947CB65FB2B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4549140" y="381000"/>
+          <a:ext cx="6187976" cy="1257409"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,7 +575,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="D3:F60"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3:E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,9 +643,18 @@
       <c r="C3" s="8">
         <v>10.276</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="D3" s="10">
+        <f>$H$1*C3+(1-$H$1)*(D2+E2)</f>
+        <v>10.2759994</v>
+      </c>
+      <c r="E3" s="10">
+        <f>$I$1*(D3-D2)+(1-$I$1)*E2</f>
+        <v>0.22196000397999974</v>
+      </c>
+      <c r="F3" s="10">
+        <f>D2+E2</f>
+        <v>10.270000000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
@@ -608,9 +666,18 @@
       <c r="C4" s="8">
         <v>10.483000000000001</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="D4" s="10">
+        <f t="shared" ref="D4:D60" si="0">$H$1*C4+(1-$H$1)*(D3+E3)</f>
+        <v>10.4830014959404</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" ref="E4:E60" si="1">$I$1*(D4-D3)+(1-$I$1)*E3</f>
+        <v>0.21707325542346242</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" ref="F4:F60" si="2">D3+E3</f>
+        <v>10.497959403979999</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
@@ -622,9 +689,18 @@
       <c r="C5" s="8">
         <v>10.742000000000001</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
+        <v>10.741995807475137</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="1"/>
+        <v>0.23076886445501585</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="2"/>
+        <v>10.700074751363863</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
@@ -636,9 +712,18 @@
       <c r="C6" s="8">
         <v>10.95</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="D6" s="10">
+        <f t="shared" si="0"/>
+        <v>10.950002276467194</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22333238985726717</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="2"/>
+        <v>10.972764671930152</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
@@ -650,9 +735,18 @@
       <c r="C7" s="8">
         <v>11.167</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
+        <v>11.167000633466632</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22126306132261447</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="2"/>
+        <v>11.173334666324461</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
@@ -664,9 +758,18 @@
       <c r="C8" s="8">
         <v>11.388</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="D8" s="10">
+        <f t="shared" si="0"/>
+        <v>11.388000026369479</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2211769208498765</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="2"/>
+        <v>11.388263694789247</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
@@ -678,9 +781,18 @@
       <c r="C9" s="8">
         <v>11.651</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="D9" s="10">
+        <f t="shared" si="0"/>
+        <v>11.650995817694723</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="1"/>
+        <v>0.23483914583417895</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="2"/>
+        <v>11.609176947219355</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
@@ -692,9 +804,18 @@
       <c r="C10" s="8">
         <v>11.798999999999999</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="D10" s="10">
+        <f t="shared" si="0"/>
+        <v>11.799008683496352</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20647300014754491</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="2"/>
+        <v>11.885834963528902</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
@@ -706,9 +827,18 @@
       <c r="C11" s="8">
         <v>12.009</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="D11" s="10">
+        <f t="shared" si="0"/>
+        <v>12.008999648168365</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20762231915768858</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="2"/>
+        <v>12.005481683643897</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
@@ -720,9 +850,18 @@
       <c r="C12" s="8">
         <v>12.263</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="D12" s="10">
+        <f t="shared" si="0"/>
+        <v>12.262995362196733</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22277250726193976</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="2"/>
+        <v>12.216621967326054</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
@@ -734,9 +873,18 @@
       <c r="C13" s="8">
         <v>12.507</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="D13" s="10">
+        <f t="shared" si="0"/>
+        <v>12.506997876786945</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22970835065608639</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="2"/>
+        <v>12.485767869458673</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
@@ -748,9 +896,18 @@
       <c r="C14" s="8">
         <v>12.936999999999999</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="D14" s="10">
+        <f t="shared" si="0"/>
+        <v>12.936979970622744</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="1"/>
+        <v>0.29513778255289835</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="2"/>
+        <v>12.736706227443031</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
@@ -762,9 +919,18 @@
       <c r="C15" s="8">
         <v>13.177</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="D15" s="10">
+        <f t="shared" si="0"/>
+        <v>13.177005511775317</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="1"/>
+        <v>0.27713261328741196</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="2"/>
+        <v>13.232117753175642</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
@@ -776,9 +942,18 @@
       <c r="C16" s="8">
         <v>13.38</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="D16" s="10">
+        <f t="shared" si="0"/>
+        <v>13.380007413812507</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2529141099219645</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="2"/>
+        <v>13.454138125062729</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
@@ -790,9 +965,18 @@
       <c r="C17" s="8">
         <v>13.723000000000001</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="D17" s="10">
+        <f t="shared" si="0"/>
+        <v>13.722990992152374</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="1"/>
+        <v>0.28233980525409319</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="2"/>
+        <v>13.632921523734471</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
@@ -804,9 +988,18 @@
       <c r="C18" s="8">
         <v>13.893000000000001</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="D18" s="10">
+        <f t="shared" si="0"/>
+        <v>13.893011233079742</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.24564500358855204</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="2"/>
+        <v>14.005330797406467</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
@@ -818,9 +1011,18 @@
       <c r="C19" s="8">
         <v>14.032999999999999</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="D19" s="10">
+        <f t="shared" si="0"/>
+        <v>14.033010565623666</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2111305628582722</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="2"/>
+        <v>14.138656236668293</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
@@ -832,9 +1034,18 @@
       <c r="C20" s="8">
         <v>14.192</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="D20" s="10">
+        <f t="shared" si="0"/>
+        <v>14.192005214112848</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="1"/>
+        <v>0.19409775963389048</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="2"/>
+        <v>14.244141128481939</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
@@ -846,9 +1057,18 @@
       <c r="C21" s="8">
         <v>14.358000000000001</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="D21" s="10">
+        <f t="shared" si="0"/>
+        <v>14.358002810297375</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="1"/>
+        <v>0.1849174362349833</v>
+      </c>
+      <c r="F21" s="10">
+        <f t="shared" si="2"/>
+        <v>14.386102973746739</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
@@ -860,9 +1080,18 @@
       <c r="C22" s="8">
         <v>14.513999999999999</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="10">
+        <f t="shared" si="0"/>
+        <v>14.514002892024651</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="1"/>
+        <v>0.17547013651731538</v>
+      </c>
+      <c r="F22" s="10">
+        <f t="shared" si="2"/>
+        <v>14.542920246532358</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
@@ -874,9 +1103,18 @@
       <c r="C23" s="8">
         <v>14.692</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="D23" s="10">
+        <f t="shared" si="0"/>
+        <v>14.691999747302853</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="1"/>
+        <v>0.17629561553649714</v>
+      </c>
+      <c r="F23" s="10">
+        <f t="shared" si="2"/>
+        <v>14.689473028541967</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
@@ -888,9 +1126,18 @@
       <c r="C24" s="8">
         <v>14.927</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
+      <c r="D24" s="10">
+        <f t="shared" si="0"/>
+        <v>14.926994129536283</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" si="1"/>
+        <v>0.19547250261638488</v>
+      </c>
+      <c r="F24" s="10">
+        <f t="shared" si="2"/>
+        <v>14.868295362839351</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
@@ -902,9 +1149,18 @@
       <c r="C25" s="8">
         <v>15.178000000000001</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
+      <c r="D25" s="10">
+        <f t="shared" si="0"/>
+        <v>15.177994446663215</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="1"/>
+        <v>0.21361343961698068</v>
+      </c>
+      <c r="F25" s="10">
+        <f t="shared" si="2"/>
+        <v>15.122466632152667</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
@@ -916,9 +1172,18 @@
       <c r="C26" s="8">
         <v>15.369</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
+      <c r="D26" s="10">
+        <f t="shared" si="0"/>
+        <v>15.369002260788628</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20622818176888558</v>
+      </c>
+      <c r="F26" s="10">
+        <f t="shared" si="2"/>
+        <v>15.391607886280196</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
@@ -930,9 +1195,18 @@
       <c r="C27" s="8">
         <v>15.544</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
+      <c r="D27" s="10">
+        <f t="shared" si="0"/>
+        <v>15.544003123044256</v>
+      </c>
+      <c r="E27" s="10">
+        <f t="shared" si="1"/>
+        <v>0.1960262164839042</v>
+      </c>
+      <c r="F27" s="10">
+        <f t="shared" si="2"/>
+        <v>15.575230442557514</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
@@ -944,9 +1218,18 @@
       <c r="C28" s="8">
         <v>15.757999999999999</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
+      <c r="D28" s="10">
+        <f t="shared" si="0"/>
+        <v>15.757998202933953</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20189664415857678</v>
+      </c>
+      <c r="F28" s="10">
+        <f t="shared" si="2"/>
+        <v>15.74002933952816</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
@@ -958,9 +1241,18 @@
       <c r="C29" s="8">
         <v>16.018000000000001</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="D29" s="10">
+        <f t="shared" si="0"/>
+        <v>16.01799418948471</v>
+      </c>
+      <c r="E29" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22087769931810222</v>
+      </c>
+      <c r="F29" s="10">
+        <f t="shared" si="2"/>
+        <v>15.95989484709253</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
@@ -972,9 +1264,18 @@
       <c r="C30" s="8">
         <v>16.263999999999999</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="D30" s="10">
+        <f t="shared" si="0"/>
+        <v>16.263997487188881</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22908623231083075</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="2"/>
+        <v>16.238871888802812</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
@@ -986,9 +1287,18 @@
       <c r="C31" s="8">
         <v>16.532</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="D31" s="10">
+        <f t="shared" si="0"/>
+        <v>16.531996108371949</v>
+      </c>
+      <c r="E31" s="10">
+        <f t="shared" si="1"/>
+        <v>0.24179890975539067</v>
+      </c>
+      <c r="F31" s="10">
+        <f t="shared" si="2"/>
+        <v>16.493083719499712</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
@@ -1000,9 +1310,18 @@
       <c r="C32" s="8">
         <v>16.814</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="D32" s="10">
+        <f t="shared" si="0"/>
+        <v>16.813995979501815</v>
+      </c>
+      <c r="E32" s="10">
+        <f t="shared" si="1"/>
+        <v>0.25493256383643176</v>
+      </c>
+      <c r="F32" s="10">
+        <f t="shared" si="2"/>
+        <v>16.773795018127341</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
@@ -1014,9 +1333,18 @@
       <c r="C33" s="8">
         <v>17.065000000000001</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
+      <c r="D33" s="10">
+        <f t="shared" si="0"/>
+        <v>17.065000392854333</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" si="1"/>
+        <v>0.25364923707333725</v>
+      </c>
+      <c r="F33" s="10">
+        <f t="shared" si="2"/>
+        <v>17.068928543338245</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9">
@@ -1028,9 +1356,18 @@
       <c r="C34" s="8">
         <v>17.283999999999999</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
+      <c r="D34" s="10">
+        <f t="shared" si="0"/>
+        <v>17.284003464962989</v>
+      </c>
+      <c r="E34" s="10">
+        <f t="shared" si="1"/>
+        <v>0.24233033497937584</v>
+      </c>
+      <c r="F34" s="10">
+        <f t="shared" si="2"/>
+        <v>17.31864962992767</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9">
@@ -1042,9 +1379,18 @@
       <c r="C35" s="8">
         <v>17.495000000000001</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
+      <c r="D35" s="10">
+        <f t="shared" si="0"/>
+        <v>17.495003133379996</v>
+      </c>
+      <c r="E35" s="10">
+        <f t="shared" si="1"/>
+        <v>0.23209460621344974</v>
+      </c>
+      <c r="F35" s="10">
+        <f t="shared" si="2"/>
+        <v>17.526333799942364</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9">
@@ -1056,9 +1402,18 @@
       <c r="C36" s="8">
         <v>17.667000000000002</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
+      <c r="D36" s="10">
+        <f t="shared" si="0"/>
+        <v>17.66700600977396</v>
+      </c>
+      <c r="E36" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2124626380814239</v>
+      </c>
+      <c r="F36" s="10">
+        <f t="shared" si="2"/>
+        <v>17.727097739593447</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9">
@@ -1070,9 +1425,18 @@
       <c r="C37" s="8">
         <v>17.855</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
+      <c r="D37" s="10">
+        <f t="shared" si="0"/>
+        <v>17.855002446864784</v>
+      </c>
+      <c r="E37" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20446953021779493</v>
+      </c>
+      <c r="F37" s="10">
+        <f t="shared" si="2"/>
+        <v>17.879468647855383</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9">
@@ -1084,9 +1448,18 @@
       <c r="C38" s="8">
         <v>18.071999999999999</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
+      <c r="D38" s="10">
+        <f t="shared" si="0"/>
+        <v>18.071998747197711</v>
+      </c>
+      <c r="E38" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20856202601440843</v>
+      </c>
+      <c r="F38" s="10">
+        <f t="shared" si="2"/>
+        <v>18.05947197708258</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
@@ -1098,9 +1471,18 @@
       <c r="C39" s="8">
         <v>18.311</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
+      <c r="D39" s="10">
+        <f t="shared" si="0"/>
+        <v>18.310996956077322</v>
+      </c>
+      <c r="E39" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2185055269564701</v>
+      </c>
+      <c r="F39" s="10">
+        <f t="shared" si="2"/>
+        <v>18.28056077321212</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9">
@@ -1112,9 +1494,18 @@
       <c r="C40" s="8">
         <v>18.516999999999999</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
+      <c r="D40" s="10">
+        <f t="shared" si="0"/>
+        <v>18.517001250248303</v>
+      </c>
+      <c r="E40" s="10">
+        <f t="shared" si="1"/>
+        <v>0.21442137420545079</v>
+      </c>
+      <c r="F40" s="10">
+        <f t="shared" si="2"/>
+        <v>18.529502483033792</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9">
@@ -1126,9 +1517,18 @@
       <c r="C41" s="8">
         <v>18.710999999999999</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
+      <c r="D41" s="10">
+        <f t="shared" si="0"/>
+        <v>18.711002042262443</v>
+      </c>
+      <c r="E41" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20774997000354969</v>
+      </c>
+      <c r="F41" s="10">
+        <f t="shared" si="2"/>
+        <v>18.731422624453753</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9">
@@ -1140,9 +1540,18 @@
       <c r="C42" s="8">
         <v>18.925999999999998</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
+      <c r="D42" s="10">
+        <f t="shared" si="0"/>
+        <v>18.925999275201224</v>
+      </c>
+      <c r="E42" s="10">
+        <f t="shared" si="1"/>
+        <v>0.21011765080448994</v>
+      </c>
+      <c r="F42" s="10">
+        <f t="shared" si="2"/>
+        <v>18.918752012265994</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9">
@@ -1154,9 +1563,18 @@
       <c r="C43" s="8">
         <v>19.152999999999999</v>
       </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
+      <c r="D43" s="10">
+        <f t="shared" si="0"/>
+        <v>19.152998311692599</v>
+      </c>
+      <c r="E43" s="10">
+        <f t="shared" si="1"/>
+        <v>0.21563279950839515</v>
+      </c>
+      <c r="F43" s="10">
+        <f t="shared" si="2"/>
+        <v>19.136116926005716</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9">
@@ -1168,9 +1586,18 @@
       <c r="C44" s="8">
         <v>19.413</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
+      <c r="D44" s="10">
+        <f t="shared" si="0"/>
+        <v>19.412995563111121</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" si="1"/>
+        <v>0.23012666594743353</v>
+      </c>
+      <c r="F44" s="10">
+        <f t="shared" si="2"/>
+        <v>19.368631111200994</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9">
@@ -1182,9 +1609,18 @@
       <c r="C45" s="8">
         <v>19.651</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
+      <c r="D45" s="10">
+        <f t="shared" si="0"/>
+        <v>19.650999212222906</v>
+      </c>
+      <c r="E45" s="10">
+        <f t="shared" si="1"/>
+        <v>0.23270007634722734</v>
+      </c>
+      <c r="F45" s="10">
+        <f t="shared" si="2"/>
+        <v>19.643122229058555</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9">
@@ -1196,9 +1632,18 @@
       <c r="C46" s="8">
         <v>19.895</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
+      <c r="D46" s="10">
+        <f t="shared" si="0"/>
+        <v>19.894998869928855</v>
+      </c>
+      <c r="E46" s="10">
+        <f t="shared" si="1"/>
+        <v>0.23639164957712167</v>
+      </c>
+      <c r="F46" s="10">
+        <f t="shared" si="2"/>
+        <v>19.883699288570135</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9">
@@ -1210,9 +1655,18 @@
       <c r="C47" s="8">
         <v>20.126999999999999</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
+      <c r="D47" s="10">
+        <f t="shared" si="0"/>
+        <v>20.127000439051951</v>
+      </c>
+      <c r="E47" s="10">
+        <f t="shared" si="1"/>
+        <v>0.23495741029279138</v>
+      </c>
+      <c r="F47" s="10">
+        <f t="shared" si="2"/>
+        <v>20.131390519505977</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9">
@@ -1224,9 +1678,18 @@
       <c r="C48" s="8">
         <v>20.395</v>
       </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
+      <c r="D48" s="10">
+        <f t="shared" si="0"/>
+        <v>20.394996695784936</v>
+      </c>
+      <c r="E48" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2457512014248027</v>
+      </c>
+      <c r="F48" s="10">
+        <f t="shared" si="2"/>
+        <v>20.361957849344741</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9">
@@ -1238,9 +1701,18 @@
       <c r="C49" s="8">
         <v>20.698</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
+      <c r="D49" s="10">
+        <f t="shared" si="0"/>
+        <v>20.697994274789721</v>
+      </c>
+      <c r="E49" s="10">
+        <f t="shared" si="1"/>
+        <v>0.26445359298018289</v>
+      </c>
+      <c r="F49" s="10">
+        <f t="shared" si="2"/>
+        <v>20.640747897209739</v>
+      </c>
     </row>
     <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9">
@@ -1252,9 +1724,18 @@
       <c r="C50" s="8">
         <v>20.827999999999999</v>
       </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
+      <c r="D50" s="10">
+        <f t="shared" si="0"/>
+        <v>20.828013444786777</v>
+      </c>
+      <c r="E50" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22053386699159516</v>
+      </c>
+      <c r="F50" s="10">
+        <f t="shared" si="2"/>
+        <v>20.962447867769903</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9">
@@ -1266,9 +1747,18 @@
       <c r="C51" s="8">
         <v>21.248999999999999</v>
       </c>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
+      <c r="D51" s="10">
+        <f t="shared" si="0"/>
+        <v>21.24897995473118</v>
+      </c>
+      <c r="E51" s="10">
+        <f t="shared" si="1"/>
+        <v>0.28601521144427755</v>
+      </c>
+      <c r="F51" s="10">
+        <f t="shared" si="2"/>
+        <v>21.048547311778371</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9">
@@ -1280,9 +1770,18 @@
       <c r="C52" s="8">
         <v>21.692</v>
       </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
+      <c r="D52" s="10">
+        <f t="shared" si="0"/>
+        <v>21.691984299516616</v>
+      </c>
+      <c r="E52" s="10">
+        <f t="shared" si="1"/>
+        <v>0.33730356130683403</v>
+      </c>
+      <c r="F52" s="10">
+        <f t="shared" si="2"/>
+        <v>21.534995166175456</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9">
@@ -1294,9 +1793,18 @@
       <c r="C53" s="8">
         <v>22.032</v>
       </c>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
+      <c r="D53" s="10">
+        <f t="shared" si="0"/>
+        <v>22.031999728786083</v>
+      </c>
+      <c r="E53" s="10">
+        <f t="shared" si="1"/>
+        <v>0.33818952857022633</v>
+      </c>
+      <c r="F53" s="10">
+        <f t="shared" si="2"/>
+        <v>22.029287860823448</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9">
@@ -1308,9 +1816,18 @@
       <c r="C54" s="8">
         <v>22.34</v>
       </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
+      <c r="D54" s="10">
+        <f t="shared" si="0"/>
+        <v>22.340003018925735</v>
+      </c>
+      <c r="E54" s="10">
+        <f t="shared" si="1"/>
+        <v>0.32832768447495775</v>
+      </c>
+      <c r="F54" s="10">
+        <f t="shared" si="2"/>
+        <v>22.370189257356309</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9">
@@ -1322,9 +1839,18 @@
       <c r="C55" s="8">
         <v>22.742000000000001</v>
       </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
+      <c r="D55" s="10">
+        <f t="shared" si="0"/>
+        <v>22.741992633070343</v>
+      </c>
+      <c r="E55" s="10">
+        <f t="shared" si="1"/>
+        <v>0.35239303689803236</v>
+      </c>
+      <c r="F55" s="10">
+        <f t="shared" si="2"/>
+        <v>22.668330703400692</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9">
@@ -1336,9 +1862,18 @@
       <c r="C56" s="8">
         <v>23.146000000000001</v>
       </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
+      <c r="D56" s="10">
+        <f t="shared" si="0"/>
+        <v>23.145994838566999</v>
+      </c>
+      <c r="E56" s="10">
+        <f t="shared" si="1"/>
+        <v>0.36925375227920282</v>
+      </c>
+      <c r="F56" s="10">
+        <f t="shared" si="2"/>
+        <v>23.094385669968375</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9">
@@ -1350,9 +1885,18 @@
       <c r="C57" s="8">
         <v>23.504000000000001</v>
       </c>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
+      <c r="D57" s="10">
+        <f t="shared" si="0"/>
+        <v>23.504001124859084</v>
+      </c>
+      <c r="E57" s="10">
+        <f t="shared" si="1"/>
+        <v>0.36557920514121134</v>
+      </c>
+      <c r="F57" s="10">
+        <f t="shared" si="2"/>
+        <v>23.515248590846202</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9">
@@ -1364,9 +1908,18 @@
       <c r="C58" s="8">
         <v>23.850999999999999</v>
       </c>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
+      <c r="D58" s="10">
+        <f t="shared" si="0"/>
+        <v>23.851001858032998</v>
+      </c>
+      <c r="E58" s="10">
+        <f t="shared" si="1"/>
+        <v>0.3595096183494953</v>
+      </c>
+      <c r="F58" s="10">
+        <f t="shared" si="2"/>
+        <v>23.869580330000296</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9">
@@ -1378,9 +1931,18 @@
       <c r="C59" s="8">
         <v>24.210999999999999</v>
       </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
+      <c r="D59" s="10">
+        <f t="shared" si="0"/>
+        <v>24.210999951147638</v>
+      </c>
+      <c r="E59" s="10">
+        <f t="shared" si="1"/>
+        <v>0.35966920305526823</v>
+      </c>
+      <c r="F59" s="10">
+        <f t="shared" si="2"/>
+        <v>24.210511476382493</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9">
@@ -1392,9 +1954,18 @@
       <c r="C60" s="8">
         <v>24.599</v>
       </c>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
+      <c r="D60" s="10">
+        <f t="shared" si="0"/>
+        <v>24.598997166915421</v>
+      </c>
+      <c r="E60" s="10">
+        <f t="shared" si="1"/>
+        <v>0.36892396480844669</v>
+      </c>
+      <c r="F60" s="10">
+        <f t="shared" si="2"/>
+        <v>24.570669154202907</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="62" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1600,5 +2171,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>